<commit_message>
Done with RVis2 - The final one
</commit_message>
<xml_diff>
--- a/r/Costof1GBofData.xlsx
+++ b/r/Costof1GBofData.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Country</t>
   </si>
   <si>
-    <t xml:space="preserve">Avg Price of 1GB (USD)</t>
+    <t xml:space="preserve">AP</t>
   </si>
   <si>
     <t xml:space="preserve">India</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Kazakhstan</t>
   </si>
   <si>
-    <t xml:space="preserve">Somalia</t>
+    <t xml:space="preserve">Somaliland</t>
   </si>
   <si>
     <t xml:space="preserve">Sri Lanka</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">Azerbaijan</t>
   </si>
   <si>
-    <t xml:space="preserve">Congo</t>
+    <t xml:space="preserve">Dem. Rep. Congo</t>
   </si>
   <si>
     <t xml:space="preserve">Sweden</t>
@@ -367,7 +367,7 @@
     <t xml:space="preserve">Mali</t>
   </si>
   <si>
-    <t xml:space="preserve">Laos</t>
+    <t xml:space="preserve">Lao PDR</t>
   </si>
   <si>
     <t xml:space="preserve">Iraq</t>
@@ -439,10 +439,10 @@
     <t xml:space="preserve">Panama</t>
   </si>
   <si>
-    <t xml:space="preserve">Czechia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States of America</t>
+    <t xml:space="preserve">Czech Rep.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States</t>
   </si>
   <si>
     <t xml:space="preserve">Central African Rep.</t>
@@ -457,7 +457,7 @@
     <t xml:space="preserve">Puerto Rico</t>
   </si>
   <si>
-    <t xml:space="preserve">South Korea</t>
+    <t xml:space="preserve">Korea</t>
   </si>
   <si>
     <t xml:space="preserve">Turkmenistan</t>
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B150" activeCellId="0" sqref="B150"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2127,7 +2127,7 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="n">
         <v>138</v>
       </c>

</xml_diff>